<commit_message>
Fix up Yolanda and Inst. Curie
</commit_message>
<xml_diff>
--- a/11-CollaborationList/CNRS-Institut-Curie.xlsx
+++ b/11-CollaborationList/CNRS-Institut-Curie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longkr/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04135C17-6468-BB42-8B6E-8B7A71897B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20A5597-E5C3-D84D-AD97-3E831005233E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{AD094988-A457-9044-86A1-58DE43D24A21}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Title</t>
   </si>
@@ -70,24 +70,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Dr.</t>
-  </si>
-  <si>
-    <t>Yolanda</t>
-  </si>
-  <si>
-    <t>Prezado</t>
-  </si>
-  <si>
-    <t>Y.</t>
-  </si>
-  <si>
-    <t>yolanda.prezado@curie.fr</t>
-  </si>
-  <si>
-    <t>Yolanda Prezado</t>
-  </si>
-  <si>
     <t>Inst-Curie</t>
   </si>
   <si>
@@ -100,18 +82,6 @@
     <t>Institut Curie, Universit PSL, CNRS UMR3347, Inserm U1021, Signalisation Radiobiologie et Cancer, 91400 Orsay, France</t>
   </si>
   <si>
-    <t>USC</t>
-  </si>
-  <si>
-    <t>University of Santiago de Compostela, Center for Research in Molecular Medicine and Chronic diseases, 15782, Santiago de Compostela, Spain</t>
-  </si>
-  <si>
-    <t>0000-0001-5957-2327</t>
-  </si>
-  <si>
-    <t>IB</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -128,36 +98,6 @@
   </si>
   <si>
     <t>Alfredo Fernandez-Rodriguez</t>
-  </si>
-  <si>
-    <t>Thongchai</t>
-  </si>
-  <si>
-    <t>Masilela</t>
-  </si>
-  <si>
-    <t>T.</t>
-  </si>
-  <si>
-    <t>thongchai.masilela@CURIE.FR</t>
-  </si>
-  <si>
-    <t>Thongchai Masilela</t>
-  </si>
-  <si>
-    <t>Frederic</t>
-  </si>
-  <si>
-    <t>Pouzoulet</t>
-  </si>
-  <si>
-    <t>F.</t>
-  </si>
-  <si>
-    <t>Frederic.Pouzoulet@CURIE.FR</t>
-  </si>
-  <si>
-    <t>Frederic Pouzoulet</t>
   </si>
 </sst>
 </file>
@@ -702,8 +642,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA1028E5-9ABD-124A-9518-518C08DAD92B}" name="Table1" displayName="Table1" ref="A1:P5" totalsRowShown="0">
-  <autoFilter ref="A1:P5" xr:uid="{DA1028E5-9ABD-124A-9518-518C08DAD92B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA1028E5-9ABD-124A-9518-518C08DAD92B}" name="Table1" displayName="Table1" ref="A1:P2" totalsRowShown="0">
+  <autoFilter ref="A1:P2" xr:uid="{DA1028E5-9ABD-124A-9518-518C08DAD92B}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{BB6016B1-80C3-E040-ABB1-1C3A7E24E79B}" name="Title"/>
     <tableColumn id="2" xr3:uid="{BD477CE4-93B2-A64E-ACFA-C9F73A744C43}" name="Name"/>
@@ -1043,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DBDFDB-9E47-924E-BB85-AA0F5297078D}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,136 +1061,37 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>